<commit_message>
backtest template added and sample file updated
</commit_message>
<xml_diff>
--- a/tests/data/sample.xlsx
+++ b/tests/data/sample.xlsx
@@ -59,6 +59,20 @@
           </rPr>
           <t xml:space="preserve">machine:
 This is manually adjusted for each strategy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">machine:
+To adjust stop loss manually for each strategy</t>
         </r>
       </text>
     </comment>
@@ -301,12 +315,12 @@
   <numFmts count="8">
     <numFmt numFmtId="176" formatCode="0_ "/>
     <numFmt numFmtId="177" formatCode="yyyy\-m\-d"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="0.000_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="0.00_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="0.00_ "/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="181" formatCode="0.000_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -327,7 +341,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -338,29 +352,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -387,8 +378,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -402,8 +438,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -416,14 +453,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -431,24 +460,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -462,8 +475,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -484,7 +498,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,7 +510,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,91 +648,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,67 +666,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -790,16 +804,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -814,11 +828,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -862,21 +882,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -887,150 +892,159 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1047,10 +1061,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1098,7 +1112,7 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -4120,9 +4134,9 @@
   <dimension ref="A1:AG39"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="AD36" sqref="AD36"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4134,17 +4148,17 @@
     <col min="8" max="8" width="8.625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="9" max="11" width="9" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="12" max="12" width="9.33333333333333" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="7.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="6.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="8.5" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="6.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="5.68333333333333" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="4.85" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="7.875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="5.875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="8.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="7.875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="7.25" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="7.25" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="6.375" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="8.5" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="6.375" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="5.68333333333333" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="4.85" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="7.875" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="5.875" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="8.375" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="7.875" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="7.25" customWidth="1"/>
     <col min="26" max="26" width="7.05833333333333" customWidth="1"/>
     <col min="27" max="27" width="7.75833333333333" customWidth="1"/>
     <col min="28" max="28" width="5.125" customWidth="1"/>
@@ -8994,10 +9008,10 @@
   <sheetPr/>
   <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="N1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="Q1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="R11" sqref="R11"/>
+      <selection pane="bottomLeft" activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>

</xml_diff>